<commit_message>
July 2013 - updated spreadsheet
</commit_message>
<xml_diff>
--- a/images/SterlingEquity.xlsx
+++ b/images/SterlingEquity.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="30" windowWidth="19140" windowHeight="9795"/>
+    <workbookView xWindow="96" yWindow="36" windowWidth="19140" windowHeight="9792"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Period</t>
   </si>
@@ -49,19 +49,16 @@
     <t>Relative Performance</t>
   </si>
   <si>
-    <t>Half Year</t>
-  </si>
-  <si>
     <t>Annualised Performance</t>
   </si>
   <si>
-    <t>16.9%pa</t>
-  </si>
-  <si>
-    <t>13.9%pa</t>
-  </si>
-  <si>
-    <t>3.0%pa</t>
+    <t>17.0% pa</t>
+  </si>
+  <si>
+    <t>3.5% pa</t>
+  </si>
+  <si>
+    <t>13.5% pa</t>
   </si>
 </sst>
 </file>
@@ -199,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -254,20 +251,11 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,21 +560,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="12.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="37.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -626,13 +614,13 @@
         <v>39629</v>
       </c>
       <c r="C3" s="10">
-        <v>-5.8999999999999997E-2</v>
+        <v>-5.8000000000000003E-2</v>
       </c>
       <c r="D3" s="13">
-        <v>-0.13700000000000001</v>
+        <v>-0.127</v>
       </c>
       <c r="E3" s="13">
-        <v>7.8E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -643,10 +631,10 @@
         <v>39994</v>
       </c>
       <c r="C4" s="10">
-        <v>0.36099999999999999</v>
+        <v>0.36199999999999999</v>
       </c>
       <c r="D4" s="13">
-        <v>-0.20300000000000001</v>
+        <v>-0.193</v>
       </c>
       <c r="E4" s="13">
         <v>0.55500000000000005</v>
@@ -703,68 +691,68 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="19">
+        <v>41455</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0.219</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="23">
-        <v>41274</v>
-      </c>
-      <c r="C8" s="10">
-        <v>0.19</v>
-      </c>
-      <c r="D8" s="13">
-        <v>0.161</v>
-      </c>
-      <c r="E8" s="13">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="11" t="s">
+      <c r="D9" s="21" t="s">
         <v>8</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>10</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="24"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="12">
-        <v>1.76</v>
-      </c>
-      <c r="D11" s="21">
-        <v>0.21</v>
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0.27</v>
       </c>
       <c r="E11" s="12">
-        <v>1.54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -787,7 +775,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -799,7 +787,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated performance table as requested
</commit_message>
<xml_diff>
--- a/images/SterlingEquity.xlsx
+++ b/images/SterlingEquity.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="36" windowWidth="19140" windowHeight="9792"/>
+    <workbookView xWindow="90" yWindow="30" windowWidth="19140" windowHeight="9795"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -251,11 +251,11 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,21 +560,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="12.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="37.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -614,13 +614,13 @@
         <v>39629</v>
       </c>
       <c r="C3" s="10">
-        <v>-5.8000000000000003E-2</v>
+        <v>-5.8999999999999997E-2</v>
       </c>
       <c r="D3" s="13">
-        <v>-0.127</v>
+        <v>-0.13700000000000001</v>
       </c>
       <c r="E3" s="13">
-        <v>6.9000000000000006E-2</v>
+        <v>7.8E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -631,13 +631,13 @@
         <v>39994</v>
       </c>
       <c r="C4" s="10">
-        <v>0.36199999999999999</v>
+        <v>0.36099999999999999</v>
       </c>
       <c r="D4" s="13">
-        <v>-0.193</v>
+        <v>-0.20300000000000001</v>
       </c>
       <c r="E4" s="13">
-        <v>0.55500000000000005</v>
+        <v>0.56499999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -708,33 +708,33 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="20"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A11" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="20"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="12">
         <v>2.0099999999999998</v>
       </c>
@@ -745,14 +745,14 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -775,7 +775,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -787,7 +787,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Jan 2014 updates as requested
</commit_message>
<xml_diff>
--- a/images/SterlingEquity.xlsx
+++ b/images/SterlingEquity.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepositories\GitHub\sterlingequity.github.com\images\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="90" yWindow="30" windowWidth="19140" windowHeight="9795"/>
+    <workbookView xWindow="96" yWindow="36" windowWidth="19140" windowHeight="9792"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Period</t>
   </si>
@@ -52,13 +57,16 @@
     <t>Annualised Performance</t>
   </si>
   <si>
-    <t>17.0% pa</t>
-  </si>
-  <si>
-    <t>3.5% pa</t>
-  </si>
-  <si>
-    <t>13.5% pa</t>
+    <t>19.3% pa</t>
+  </si>
+  <si>
+    <t>5.1% pa</t>
+  </si>
+  <si>
+    <t>14.2% pa</t>
+  </si>
+  <si>
+    <t>Half Year to</t>
   </si>
 </sst>
 </file>
@@ -267,6 +275,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -314,7 +325,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -349,7 +360,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -558,23 +569,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="12.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="37.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -708,61 +719,78 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="21" t="s">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="19">
+        <v>41639</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="11" t="s">
+      <c r="B10" s="21"/>
+      <c r="C10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E10" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A11" s="21" t="s">
+    <row r="11" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="12">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="D11" s="12">
-        <v>0.27</v>
-      </c>
-      <c r="E11" s="12">
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A13" s="6"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="12">
+        <v>2.76</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="E12" s="12">
+        <v>2.31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -775,7 +803,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -787,7 +815,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed performance table to Times New Roman Text
</commit_message>
<xml_diff>
--- a/images/SterlingEquity.xlsx
+++ b/images/SterlingEquity.xlsx
@@ -32,6 +32,27 @@
     <t>Cumulative Performance</t>
   </si>
   <si>
+    <t>S&amp;P ASX 300 Acc. Index</t>
+  </si>
+  <si>
+    <t>Relative Performance</t>
+  </si>
+  <si>
+    <t>Annualised Performance</t>
+  </si>
+  <si>
+    <t>19.3% pa</t>
+  </si>
+  <si>
+    <t>5.1% pa</t>
+  </si>
+  <si>
+    <t>14.2% pa</t>
+  </si>
+  <si>
+    <t>Half Year to</t>
+  </si>
+  <si>
     <r>
       <t>Sterling Equity returns after fees</t>
     </r>
@@ -41,32 +62,11 @@
         <vertAlign val="superscript"/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Perpetua"/>
+        <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
       <t>2</t>
     </r>
-  </si>
-  <si>
-    <t>S&amp;P ASX 300 Acc. Index</t>
-  </si>
-  <si>
-    <t>Relative Performance</t>
-  </si>
-  <si>
-    <t>Annualised Performance</t>
-  </si>
-  <si>
-    <t>19.3% pa</t>
-  </si>
-  <si>
-    <t>5.1% pa</t>
-  </si>
-  <si>
-    <t>14.2% pa</t>
-  </si>
-  <si>
-    <t>Half Year to</t>
   </si>
 </sst>
 </file>
@@ -77,7 +77,7 @@
     <numFmt numFmtId="164" formatCode="d\ mmmm\ yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,10 +100,23 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Perpetua"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
     </font>
   </fonts>
@@ -204,66 +217,69 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,12 +588,12 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E12" sqref="A1:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.44140625" style="1" customWidth="1"/>
@@ -585,207 +601,207 @@
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:5" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10">
+        <v>39263</v>
+      </c>
+      <c r="C2" s="11">
+        <v>0.31</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="E2" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13">
+        <v>39629</v>
+      </c>
+      <c r="C3" s="14">
+        <v>-5.8999999999999997E-2</v>
+      </c>
+      <c r="D3" s="15">
+        <v>-0.13700000000000001</v>
+      </c>
+      <c r="E3" s="15">
+        <v>7.8E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13">
+        <v>39994</v>
+      </c>
+      <c r="C4" s="14">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="D4" s="15">
+        <v>-0.20300000000000001</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0.56499999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13">
+        <v>40359</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13">
+        <v>40724</v>
+      </c>
+      <c r="C6" s="14">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="D6" s="15">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="E6" s="15">
+        <v>-3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13">
+        <v>41090</v>
+      </c>
+      <c r="C7" s="14">
+        <v>-3.6999999999999998E-2</v>
+      </c>
+      <c r="D7" s="15">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="E7" s="15">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="13">
+        <v>41455</v>
+      </c>
+      <c r="C8" s="14">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="D8" s="15">
+        <v>0.219</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="13">
+        <v>41639</v>
+      </c>
+      <c r="C9" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D9" s="15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E9" s="15">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="18">
-        <v>39263</v>
-      </c>
-      <c r="C2" s="15">
-        <v>0.31</v>
-      </c>
-      <c r="D2" s="16">
-        <v>0.29199999999999998</v>
-      </c>
-      <c r="E2" s="16">
-        <v>1.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="19">
-        <v>39629</v>
-      </c>
-      <c r="C3" s="10">
-        <v>-5.8999999999999997E-2</v>
-      </c>
-      <c r="D3" s="13">
-        <v>-0.13700000000000001</v>
-      </c>
-      <c r="E3" s="13">
-        <v>7.8E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="19">
-        <v>39994</v>
-      </c>
-      <c r="C4" s="10">
-        <v>0.36099999999999999</v>
-      </c>
-      <c r="D4" s="13">
-        <v>-0.20300000000000001</v>
-      </c>
-      <c r="E4" s="13">
-        <v>0.56499999999999995</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="19">
-        <v>40359</v>
-      </c>
-      <c r="C5" s="10">
-        <v>0.32200000000000001</v>
-      </c>
-      <c r="D5" s="13">
-        <v>0.13100000000000001</v>
-      </c>
-      <c r="E5" s="13">
-        <v>0.192</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="19">
-        <v>40724</v>
-      </c>
-      <c r="C6" s="10">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="D6" s="13">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="E6" s="13">
-        <v>-3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="19">
-        <v>41090</v>
-      </c>
-      <c r="C7" s="10">
-        <v>-3.6999999999999998E-2</v>
-      </c>
-      <c r="D7" s="13">
-        <v>-7.0000000000000007E-2</v>
-      </c>
-      <c r="E7" s="13">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="19">
-        <v>41455</v>
-      </c>
-      <c r="C8" s="10">
-        <v>0.29899999999999999</v>
-      </c>
-      <c r="D8" s="13">
-        <v>0.219</v>
-      </c>
-      <c r="E8" s="13">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="19">
-        <v>41639</v>
-      </c>
-      <c r="C9" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="D9" s="13">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E9" s="13">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="11" t="s">
+      <c r="D10" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="E10" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="12">
+      <c r="B12" s="16"/>
+      <c r="C12" s="22">
         <v>2.76</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="22">
         <v>0.45</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="22">
         <v>2.31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
June 30 2016 updates
</commit_message>
<xml_diff>
--- a/images/SterlingEquity.xlsx
+++ b/images/SterlingEquity.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>Period</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>Annualised Performance</t>
-  </si>
-  <si>
-    <t>9 Months to</t>
   </si>
   <si>
     <t>S&amp;P ASX 300 Acc. Index (%)</t>
@@ -73,10 +70,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\ mmmm\ yyyy"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -129,7 +126,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -205,20 +202,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -249,40 +237,34 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -378,6 +360,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -413,6 +412,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -589,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -611,13 +627,13 @@
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -627,13 +643,13 @@
       <c r="B2" s="10">
         <v>39263</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="12">
         <v>31</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="15">
         <v>29.2</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2" s="15">
         <v>1.8</v>
       </c>
     </row>
@@ -644,13 +660,13 @@
       <c r="B3" s="11">
         <v>39629</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="13">
         <v>-5.9</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="16">
         <v>-13.7</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="16">
         <v>7.8</v>
       </c>
     </row>
@@ -661,13 +677,13 @@
       <c r="B4" s="11">
         <v>39994</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="13">
         <v>36.1</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="16">
         <v>-20.3</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="16">
         <v>56.5</v>
       </c>
     </row>
@@ -678,13 +694,13 @@
       <c r="B5" s="11">
         <v>40359</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="13">
         <v>32.200000000000003</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="16">
         <v>13.1</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="16">
         <v>19.2</v>
       </c>
     </row>
@@ -695,13 +711,13 @@
       <c r="B6" s="11">
         <v>40724</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="13">
         <v>8.4</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="16">
         <v>11.9</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="16">
         <v>-3.5</v>
       </c>
     </row>
@@ -712,13 +728,13 @@
       <c r="B7" s="11">
         <v>41090</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="13">
         <v>-3.7</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="16">
         <v>-7</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="16">
         <v>3.3</v>
       </c>
     </row>
@@ -729,13 +745,13 @@
       <c r="B8" s="11">
         <v>41455</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="13">
         <v>29.9</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="16">
         <v>21.9</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="16">
         <v>8</v>
       </c>
     </row>
@@ -746,13 +762,13 @@
       <c r="B9" s="11">
         <v>41820</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="13">
         <v>22.2</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="16">
         <v>17.3</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="16">
         <v>5</v>
       </c>
     </row>
@@ -763,88 +779,81 @@
       <c r="B10" s="11">
         <v>42185</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="13">
         <v>6.4</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="16">
         <v>5.6</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="16">
         <v>0.8</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="14">
-        <v>42460</v>
-      </c>
-      <c r="C11" s="17">
-        <v>1.6</v>
-      </c>
-      <c r="D11" s="21">
-        <v>-3</v>
-      </c>
-      <c r="E11" s="21">
-        <v>4.5999999999999996</v>
+        <v>1</v>
+      </c>
+      <c r="B11" s="11">
+        <v>42551</v>
+      </c>
+      <c r="C11" s="13">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D11" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="16">
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="18">
-        <v>15.2</v>
-      </c>
-      <c r="D12" s="22">
-        <v>4.5</v>
-      </c>
-      <c r="E12" s="23">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="14">
+        <v>15.6</v>
+      </c>
+      <c r="D12" s="17">
+        <v>4.8</v>
+      </c>
+      <c r="E12" s="18">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="21">
+        <v>327</v>
+      </c>
+      <c r="D13" s="21">
+        <v>59</v>
+      </c>
+      <c r="E13" s="21">
+        <v>268</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="19">
-        <v>298</v>
-      </c>
-      <c r="D14" s="19">
-        <v>53</v>
-      </c>
-      <c r="E14" s="19">
-        <v>245</v>
-      </c>
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
+      <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Dec 31 2016 updates
</commit_message>
<xml_diff>
--- a/images/SterlingEquity.xlsx
+++ b/images/SterlingEquity.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
   <si>
     <t>Period</t>
   </si>
@@ -65,6 +65,9 @@
       </rPr>
       <t>(%)</t>
     </r>
+  </si>
+  <si>
+    <t>Half Year to</t>
   </si>
 </sst>
 </file>
@@ -258,14 +261,14 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,11 +608,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -806,54 +807,71 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+    <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="11">
+        <v>42735</v>
+      </c>
+      <c r="C12" s="13">
+        <v>13.6</v>
+      </c>
+      <c r="D12" s="16">
+        <v>10.4</v>
+      </c>
+      <c r="E12" s="16">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="14">
-        <v>15.6</v>
-      </c>
-      <c r="D12" s="17">
-        <v>4.8</v>
-      </c>
-      <c r="E12" s="18">
-        <v>10.9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="14">
+        <v>16.2</v>
+      </c>
+      <c r="D13" s="17">
+        <v>5.5</v>
+      </c>
+      <c r="E13" s="18">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21">
-        <v>327</v>
-      </c>
-      <c r="D13" s="21">
-        <v>59</v>
-      </c>
-      <c r="E13" s="21">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="19">
+        <v>385</v>
+      </c>
+      <c r="D14" s="19">
+        <v>76</v>
+      </c>
+      <c r="E14" s="19">
+        <v>309</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
+      <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
correct mistake on performance table
</commit_message>
<xml_diff>
--- a/images/SterlingEquity.xlsx
+++ b/images/SterlingEquity.xlsx
@@ -632,7 +632,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -857,7 +857,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="11">
-        <v>43465</v>
+        <v>43100</v>
       </c>
       <c r="C13" s="13">
         <v>17.8</v>

</xml_diff>

<commit_message>
update graph and performance table
</commit_message>
<xml_diff>
--- a/images/SterlingEquity.xlsx
+++ b/images/SterlingEquity.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\GitRepositories\sterlingequity.github.com\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E5175959-A37D-48BA-A7CA-851FAD9AC2A9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0A559C-6F3C-4B85-97F9-8C53FCB92388}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PerfTable" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>Period</t>
   </si>
@@ -627,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -867,57 +874,74 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="11">
+        <v>43646</v>
+      </c>
+      <c r="C14" s="13">
+        <v>33.5</v>
+      </c>
+      <c r="D14" s="16">
+        <v>11.4</v>
+      </c>
+      <c r="E14" s="16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="14">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="D14" s="17">
-        <v>6.2</v>
-      </c>
-      <c r="E14" s="18">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="B15" s="21"/>
+      <c r="C15" s="14">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="D15" s="17">
+        <v>6.6</v>
+      </c>
+      <c r="E15" s="18">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="19">
-        <v>552</v>
-      </c>
-      <c r="D15" s="19">
-        <v>105</v>
-      </c>
-      <c r="E15" s="19">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="23" t="s">
+      <c r="B16" s="22"/>
+      <c r="C16" s="19">
+        <v>770</v>
+      </c>
+      <c r="D16" s="19">
+        <v>129</v>
+      </c>
+      <c r="E16" s="19">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" ht="19.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>